<commit_message>
setup virtual machine and setup cluster
</commit_message>
<xml_diff>
--- a/02_requirements/SHMACK Backlog.xlsx
+++ b/02_requirements/SHMACK Backlog.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$4:$E$4</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -108,51 +111,9 @@
     <t>SM-7</t>
   </si>
   <si>
-    <t>SM-8</t>
-  </si>
-  <si>
     <t>SM-9</t>
   </si>
   <si>
-    <t>SM-10</t>
-  </si>
-  <si>
-    <t>SM-11</t>
-  </si>
-  <si>
-    <t>SM-12</t>
-  </si>
-  <si>
-    <t>SM-13</t>
-  </si>
-  <si>
-    <t>SM-14</t>
-  </si>
-  <si>
-    <t>SM-15</t>
-  </si>
-  <si>
-    <t>SM-16</t>
-  </si>
-  <si>
-    <t>SM-17</t>
-  </si>
-  <si>
-    <t>SM-18</t>
-  </si>
-  <si>
-    <t>SM-19</t>
-  </si>
-  <si>
-    <t>SM-20</t>
-  </si>
-  <si>
-    <t>SM-21</t>
-  </si>
-  <si>
-    <t>SM-22</t>
-  </si>
-  <si>
     <t>Word count</t>
   </si>
   <si>
@@ -238,6 +199,21 @@
   </si>
   <si>
     <t>2015-10-27: wgi: Security will be added later, not relevant for first puncture through all layers</t>
+  </si>
+  <si>
+    <t>Nadja Ulrich, Matthias Fuhr (Data Scientists)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machine Learning </t>
+  </si>
+  <si>
+    <t>Local Development with Spark (no Cloud)</t>
+  </si>
+  <si>
+    <t>Matching Amplab Reference Architecture</t>
+  </si>
+  <si>
+    <t>Real Time Word Cloud (Streaming)</t>
   </si>
 </sst>
 </file>
@@ -620,11 +596,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,10 +610,12 @@
     <col min="3" max="3" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="51" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="45.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -645,15 +623,15 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -667,10 +645,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -684,7 +662,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -698,200 +676,172 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="2" t="s">
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A4:E4"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -903,22 +853,22 @@
     <hyperlink ref="D8" r:id="rId5"/>
     <hyperlink ref="D10" r:id="rId6"/>
     <hyperlink ref="D13" r:id="rId7"/>
-    <hyperlink ref="D15" r:id="rId8"/>
-    <hyperlink ref="D17" r:id="rId9"/>
-    <hyperlink ref="D19" r:id="rId10"/>
-    <hyperlink ref="D21" r:id="rId11"/>
-    <hyperlink ref="D23" r:id="rId12"/>
-    <hyperlink ref="D25" r:id="rId13"/>
+    <hyperlink ref="G14" r:id="rId8"/>
+    <hyperlink ref="G16" r:id="rId9"/>
+    <hyperlink ref="G18" r:id="rId10"/>
+    <hyperlink ref="G20" r:id="rId11"/>
+    <hyperlink ref="G22" r:id="rId12"/>
+    <hyperlink ref="G24" r:id="rId13"/>
     <hyperlink ref="D7" r:id="rId14"/>
     <hyperlink ref="D9" r:id="rId15"/>
-    <hyperlink ref="D12" r:id="rId16"/>
-    <hyperlink ref="D14" r:id="rId17"/>
-    <hyperlink ref="D16" r:id="rId18"/>
-    <hyperlink ref="D18" r:id="rId19"/>
-    <hyperlink ref="D20" r:id="rId20"/>
-    <hyperlink ref="D22" r:id="rId21"/>
-    <hyperlink ref="D24" r:id="rId22"/>
-    <hyperlink ref="D26" r:id="rId23"/>
+    <hyperlink ref="G11" r:id="rId16"/>
+    <hyperlink ref="G13" r:id="rId17"/>
+    <hyperlink ref="G15" r:id="rId18"/>
+    <hyperlink ref="G17" r:id="rId19"/>
+    <hyperlink ref="G19" r:id="rId20"/>
+    <hyperlink ref="G21" r:id="rId21"/>
+    <hyperlink ref="G23" r:id="rId22"/>
+    <hyperlink ref="G25" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId24"/>

</xml_diff>

<commit_message>
SM-1 ready, added "Done" column in backlog
</commit_message>
<xml_diff>
--- a/02_requirements/SHMACK Backlog.xlsx
+++ b/02_requirements/SHMACK Backlog.xlsx
@@ -8,9 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lists" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$4:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$4:$F$4</definedName>
+    <definedName name="STATUS">Lists!$A$1:$A$3</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -214,13 +216,25 @@
   </si>
   <si>
     <t>Real Time Word Cloud (Streaming)</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Enter List values below here</t>
+  </si>
+  <si>
+    <t>Enter List values above here</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,8 +263,16 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,6 +282,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,7 +305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -291,12 +319,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -596,11 +646,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,30 +658,32 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="42.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="51" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="45.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="20.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="51" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="45.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -642,13 +694,16 @@
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -658,39 +713,42 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -700,11 +758,11 @@
       <c r="C8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -714,11 +772,11 @@
       <c r="C9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -728,11 +786,11 @@
       <c r="C10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -742,136 +800,177 @@
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G16" s="2" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="2" t="s">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="2" t="s">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="2" t="s">
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="2" t="s">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G21" s="2" t="s">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G22" s="2" t="s">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="2" t="s">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="2" t="s">
+    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G25" s="2" t="s">
+    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="2" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:E4"/>
+  <autoFilter ref="A4:F4"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1227">
+      <formula1>"STATUS"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="D5" r:id="rId2"/>
-    <hyperlink ref="D6" r:id="rId3"/>
-    <hyperlink ref="D11" r:id="rId4"/>
-    <hyperlink ref="D8" r:id="rId5"/>
-    <hyperlink ref="D10" r:id="rId6"/>
-    <hyperlink ref="D13" r:id="rId7"/>
-    <hyperlink ref="G14" r:id="rId8"/>
-    <hyperlink ref="G16" r:id="rId9"/>
-    <hyperlink ref="G18" r:id="rId10"/>
-    <hyperlink ref="G20" r:id="rId11"/>
-    <hyperlink ref="G22" r:id="rId12"/>
-    <hyperlink ref="G24" r:id="rId13"/>
-    <hyperlink ref="D7" r:id="rId14"/>
-    <hyperlink ref="D9" r:id="rId15"/>
-    <hyperlink ref="G11" r:id="rId16"/>
-    <hyperlink ref="G13" r:id="rId17"/>
-    <hyperlink ref="G15" r:id="rId18"/>
-    <hyperlink ref="G17" r:id="rId19"/>
-    <hyperlink ref="G19" r:id="rId20"/>
-    <hyperlink ref="G21" r:id="rId21"/>
-    <hyperlink ref="G23" r:id="rId22"/>
-    <hyperlink ref="G25" r:id="rId23"/>
+    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="E7" r:id="rId3"/>
+    <hyperlink ref="E11" r:id="rId4"/>
+    <hyperlink ref="E8" r:id="rId5"/>
+    <hyperlink ref="E10" r:id="rId6"/>
+    <hyperlink ref="E13" r:id="rId7"/>
+    <hyperlink ref="H14" r:id="rId8"/>
+    <hyperlink ref="H16" r:id="rId9"/>
+    <hyperlink ref="H18" r:id="rId10"/>
+    <hyperlink ref="H20" r:id="rId11"/>
+    <hyperlink ref="H22" r:id="rId12"/>
+    <hyperlink ref="H24" r:id="rId13"/>
+    <hyperlink ref="E6" r:id="rId14"/>
+    <hyperlink ref="E9" r:id="rId15"/>
+    <hyperlink ref="H11" r:id="rId16"/>
+    <hyperlink ref="H13" r:id="rId17"/>
+    <hyperlink ref="H15" r:id="rId18"/>
+    <hyperlink ref="H17" r:id="rId19"/>
+    <hyperlink ref="H19" r:id="rId20"/>
+    <hyperlink ref="H21" r:id="rId21"/>
+    <hyperlink ref="H23" r:id="rId22"/>
+    <hyperlink ref="H25" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId24"/>
   <legacyDrawing r:id="rId25"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>